<commit_message>
add and remove table params lines
</commit_message>
<xml_diff>
--- a/tasks/OctopusVer1.xlsx
+++ b/tasks/OctopusVer1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilan\github\Development\tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC33E74-A886-431F-B3D4-06371E7AFB36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EC48D9-7D93-4860-80C3-C9EAB3DB883F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4855DEEB-F248-4B1C-BB17-5DC295BB82DD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="47">
   <si>
     <t>פונקציונליות לגרסה:</t>
   </si>
@@ -96,12 +96,6 @@
     <t>בשמירה של פונקציה</t>
   </si>
   <si>
-    <t>is_class_method</t>
-  </si>
-  <si>
-    <t>class_name</t>
-  </si>
-  <si>
     <t xml:space="preserve">להוסיף 2 שדות בhtml </t>
   </si>
   <si>
@@ -169,6 +163,16 @@
   </si>
   <si>
     <t>ממשק לTFS</t>
+  </si>
+  <si>
+    <t>האובייקט של בחירת הפונקציה
+ צריך להיות מסוג dataList</t>
+  </si>
+  <si>
+    <t>is_class_method - cb</t>
+  </si>
+  <si>
+    <t>class_name - להוסיף בטופס ולהעביר כ Text  בשמירה</t>
   </si>
 </sst>
 </file>
@@ -197,7 +201,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,6 +220,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -349,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -401,6 +417,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -717,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F83257B-FE68-47AB-8406-4E389FAD5257}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="E14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -728,6 +759,7 @@
     <col min="2" max="2" width="24.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -738,7 +770,7 @@
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>1</v>
@@ -755,7 +787,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
@@ -772,7 +804,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>5</v>
@@ -788,38 +820,38 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>15</v>
@@ -832,35 +864,33 @@
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>17</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>20</v>
@@ -872,163 +902,163 @@
         <v>8</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B13" s="5"/>
       <c r="C13" s="6"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>24</v>
+      <c r="C14" s="23"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="E15" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C18" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>12</v>
-      </c>
+      <c r="D18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="15" t="s">
-        <v>39</v>
+      <c r="A20" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>40</v>
+      <c r="A21" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>12</v>
@@ -1036,14 +1066,16 @@
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="12"/>
+        <v>38</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="D22" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>12</v>
@@ -1051,47 +1083,62 @@
     </row>
     <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="16" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="18" t="s">
-        <v>42</v>
+      <c r="A24" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C27" t="s">
-        <v>31</v>
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C29" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>